<commit_message>
branch v_3: start load
</commit_message>
<xml_diff>
--- a/target/classes/universityInfo.xlsx
+++ b/target/classes/universityInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\0.MyFile\Java_Project\Maven_Gradle_01\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B72C6BF-0FDB-4B7E-8952-2F21C2C01D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB791D6B-EEDD-4FA9-88E5-379E883AC064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="197" yWindow="2194" windowWidth="12463" windowHeight="10920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="197" yWindow="2194" windowWidth="12463" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Students" sheetId="1" r:id="rId1"/>
@@ -546,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -736,7 +736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>

</xml_diff>